<commit_message>
updated readme and highlevelstats
</commit_message>
<xml_diff>
--- a/Highlevelstats.xlsx
+++ b/Highlevelstats.xlsx
@@ -16,11 +16,12 @@
     <sheet name="Raw Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Raw Data'!$A$1:$K$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Raw Data'!$B$1:$B$69</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="12" r:id="rId3"/>
+    <pivotCache cacheId="16" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="57">
   <si>
     <t>College of Arts </t>
   </si>
@@ -114,15 +115,6 @@
     <t>Arts</t>
   </si>
   <si>
-    <t xml:space="preserve"> Presentations and Public Lectures </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Theses and Dissertations </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Working Papers </t>
-  </si>
-  <si>
     <t>Business and Law</t>
   </si>
   <si>
@@ -132,9 +124,6 @@
     <t>Science</t>
   </si>
   <si>
-    <t xml:space="preserve"> Research Data </t>
-  </si>
-  <si>
     <t>Non-Academic &amp; External</t>
   </si>
   <si>
@@ -165,9 +154,6 @@
     <t>Engineering  University of Canterbury Fire Engineering Programme Research Publications </t>
   </si>
   <si>
-    <t>(Some are in more than one collection!)</t>
-  </si>
-  <si>
     <t>Reports </t>
   </si>
   <si>
@@ -178,6 +164,45 @@
   </si>
   <si>
     <t>Journal Articles </t>
+  </si>
+  <si>
+    <t>Education, Health and Human Development</t>
+  </si>
+  <si>
+    <t>Presentations and Public Lectures </t>
+  </si>
+  <si>
+    <t>Theses and Dissertations </t>
+  </si>
+  <si>
+    <t>Working Papers </t>
+  </si>
+  <si>
+    <t>Research Data </t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Green OA</t>
+  </si>
+  <si>
+    <t>Unique/Green OA</t>
+  </si>
+  <si>
+    <t>Unique - Soley held by Canterbury</t>
+  </si>
+  <si>
+    <t>NA  - Not for preservation, for internal use</t>
+  </si>
+  <si>
+    <t>Green OA - manuscript copies of material held elsewhere</t>
+  </si>
+  <si>
+    <t>Legend</t>
   </si>
 </sst>
 </file>
@@ -238,35 +263,40 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Anton Angelo" refreshedDate="43308.397429745368" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="46">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Anton Angelo" refreshedDate="43308.658302199074" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="53">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A12:C58" sheet="Raw Data"/>
+    <worksheetSource ref="A12:C65" sheet="Raw Data"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="College" numFmtId="0">
       <sharedItems/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
-      <sharedItems count="21">
+      <sharedItems count="26">
         <s v="Chapters and Books "/>
         <s v="Conference Contributions "/>
         <s v="Creative Works"/>
         <s v="Journal Articles "/>
-        <s v=" Presentations and Public Lectures "/>
+        <s v="Presentations and Public Lectures "/>
         <s v="Reports "/>
-        <s v=" Theses and Dissertations "/>
-        <s v=" Working Papers "/>
-        <s v=" Research Data "/>
+        <s v="Theses and Dissertations "/>
+        <s v="Working Papers "/>
+        <s v="Research Data "/>
         <s v="Research Centre"/>
         <s v="Repository Published Journal"/>
         <s v="UC Library administrative collection"/>
         <s v=" Centre for Advanced Engineering " u="1"/>
+        <s v=" Research Data " u="1"/>
         <s v=" Reports " u="1"/>
+        <s v=" Working Papers " u="1"/>
         <s v=" Conference Contributions " u="1"/>
         <s v=" Creative Works " u="1"/>
         <s v=" Chapters and Books " u="1"/>
         <s v="Creative Work" u="1"/>
         <s v="Reports" u="1"/>
+        <s v="Creative Works " u="1"/>
+        <s v=" Presentations and Public Lectures " u="1"/>
+        <s v=" Theses and Dissertations " u="1"/>
         <s v=" University of Canterbury Fire Engineering Programme Research Publications " u="1"/>
         <s v=" Journal Articles " u="1"/>
       </sharedItems>
@@ -283,8 +313,50 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Anton Angelo" refreshedDate="43308.661398842596" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="12">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="F1:H13" sheet="Raw Data"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Type" numFmtId="0">
+      <sharedItems count="12">
+        <s v="Repository Published Journal"/>
+        <s v="Research Centre"/>
+        <s v="UC Library administrative collection"/>
+        <s v="Creative Works"/>
+        <s v="Chapters and Books "/>
+        <s v="Conference Contributions "/>
+        <s v="Journal Articles "/>
+        <s v="Reports "/>
+        <s v="Presentations and Public Lectures "/>
+        <s v="Theses and Dissertations "/>
+        <s v="Working Papers "/>
+        <s v="Research Data "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Total" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="7983"/>
+    </cacheField>
+    <cacheField name="Type2" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Unique"/>
+        <s v="NA"/>
+        <s v="Green OA"/>
+        <s v="Unique/Green OA"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="46">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="53">
   <r>
     <s v="Arts"/>
     <x v="0"/>
@@ -371,6 +443,41 @@
     <n v="98"/>
   </r>
   <r>
+    <s v="Education, Health and Human Development"/>
+    <x v="0"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <s v="Education, Health and Human Development"/>
+    <x v="1"/>
+    <n v="235"/>
+  </r>
+  <r>
+    <s v="Education, Health and Human Development"/>
+    <x v="2"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <s v="Education, Health and Human Development"/>
+    <x v="3"/>
+    <n v="220"/>
+  </r>
+  <r>
+    <s v="Education, Health and Human Development"/>
+    <x v="4"/>
+    <n v="28"/>
+  </r>
+  <r>
+    <s v="Education, Health and Human Development"/>
+    <x v="5"/>
+    <n v="54"/>
+  </r>
+  <r>
+    <s v="Education, Health and Human Development"/>
+    <x v="6"/>
+    <n v="672"/>
+  </r>
+  <r>
     <s v="Engineering"/>
     <x v="0"/>
     <n v="20"/>
@@ -514,38 +621,175 @@
     <s v="Staging "/>
     <x v="11"/>
     <n v="22"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="12">
+  <r>
+    <x v="0"/>
+    <n v="246"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="614"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="22"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="34"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="82"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="2833"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="2130"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="1090"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="118"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="7983"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="226"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3"/>
+    <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E9:F14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField showAll="0">
+      <items count="13">
+        <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="11"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="22">
+      <items count="27">
         <item m="1" x="12"/>
+        <item m="1" x="18"/>
         <item m="1" x="16"/>
+        <item m="1" x="17"/>
+        <item m="1" x="25"/>
+        <item m="1" x="22"/>
         <item m="1" x="14"/>
+        <item m="1" x="13"/>
+        <item m="1" x="23"/>
+        <item m="1" x="24"/>
         <item m="1" x="15"/>
-        <item m="1" x="20"/>
-        <item x="4"/>
-        <item m="1" x="13"/>
-        <item x="8"/>
-        <item x="6"/>
         <item m="1" x="19"/>
-        <item x="7"/>
-        <item m="1" x="17"/>
         <item x="10"/>
         <item x="9"/>
         <item x="11"/>
         <item x="2"/>
-        <item m="1" x="18"/>
+        <item m="1" x="20"/>
         <item x="0"/>
         <item x="1"/>
         <item x="3"/>
         <item x="5"/>
+        <item m="1" x="21"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -555,18 +799,6 @@
     <field x="1"/>
   </rowFields>
   <rowItems count="13">
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
     <i>
       <x v="12"/>
     </i>
@@ -590,6 +822,18 @@
     </i>
     <i>
       <x v="20"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
     </i>
     <i t="grand">
       <x/>
@@ -873,190 +1117,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F16"/>
+  <dimension ref="A3:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="3">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2833</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2130</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="3">
+        <v>5045</v>
+      </c>
+      <c r="H10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B11" s="3">
+        <v>1090</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="3">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="3">
+        <v>118</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="3">
+        <v>8998</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="3">
+        <v>7983</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="3">
+        <v>226</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="3">
+        <v>15381</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3">
+        <v>15381</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="B18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="3">
-        <v>90</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="B19">
         <v>1913</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="3">
-        <v>7311</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="3">
-        <v>226</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7">
+      <c r="B22">
         <v>5872</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>4306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
         <v>246</v>
       </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>4306</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="3">
-        <v>614</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="3">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="3">
-        <v>74</v>
-      </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="F12">
+      <c r="B27">
         <v>15285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="3">
-        <v>2598</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1910</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="3">
-        <v>14153</v>
       </c>
     </row>
   </sheetData>
@@ -1066,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection sqref="A1:C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,79 +1392,160 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="C2">
         <v>1913</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>246</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
         <v>1033</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3">
+        <v>614</v>
+      </c>
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="C4">
         <v>1228</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="C5">
         <v>5872</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
         <v>4306</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6">
+        <v>82</v>
+      </c>
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="C7">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7">
+        <v>2833</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="C8">
         <v>614</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8">
+        <v>2130</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="C9">
         <v>246</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9">
+        <v>1090</v>
+      </c>
+      <c r="H9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1159,60 +1553,95 @@
         <f>SUM(C2:C9)</f>
         <v>15285</v>
       </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>118</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11">
+        <v>7983</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12">
+        <v>226</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C13">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>164</v>
@@ -1223,7 +1652,7 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C17">
         <v>42</v>
@@ -1234,7 +1663,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C18">
         <v>29</v>
@@ -1245,7 +1674,7 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C19">
         <v>1471</v>
@@ -1256,7 +1685,7 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C20">
         <v>16</v>
@@ -1267,7 +1696,7 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -1275,10 +1704,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -1286,10 +1715,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C23">
         <v>226</v>
@@ -1297,10 +1726,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C24">
         <v>193</v>
@@ -1308,10 +1737,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1319,10 +1748,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C26">
         <v>49</v>
@@ -1330,10 +1759,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C27">
         <v>352</v>
@@ -1341,10 +1770,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C28">
         <v>185</v>
@@ -1352,10 +1781,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C29">
         <v>98</v>
@@ -1363,330 +1792,408 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C30">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C31">
-        <v>1890</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C32">
-        <v>980</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C33">
-        <v>24</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
         <v>45</v>
       </c>
       <c r="C34">
-        <v>692</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C35">
-        <v>2131</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C36">
-        <v>98</v>
+        <v>672</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C37">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C38">
-        <v>34</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C39">
-        <v>286</v>
+        <v>980</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C40">
-        <v>573</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C41">
-        <v>53</v>
+        <v>692</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C43">
-        <v>3357</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C44">
-        <v>546</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C45">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C46">
-        <v>48</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C47">
-        <v>12</v>
+        <v>573</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C48">
-        <v>120</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C49">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C50">
-        <v>8</v>
+        <v>3357</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C51">
-        <v>62</v>
+        <v>546</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C54">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C56">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C57">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>24</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B65" t="s">
         <v>23</v>
       </c>
-      <c r="C58">
+      <c r="C65">
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C59">
-        <f>SUM(C13:C58)</f>
-        <v>14153</v>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <f>SUM(C13:C65)</f>
+        <v>15381</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B69"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>